<commit_message>
textos de la memoria, falta
</commit_message>
<xml_diff>
--- a/De que hablar.xlsx
+++ b/De que hablar.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="que poner" sheetId="1" r:id="rId1"/>
+    <sheet name="memorias" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>IED</t>
   </si>
@@ -109,6 +110,96 @@
   </si>
   <si>
     <t>Hablar de principales Acreedores y a qué sectores se dirigen sus desembolsos</t>
+  </si>
+  <si>
+    <t>Crecimiento</t>
+  </si>
+  <si>
+    <t>Crecimiento en relación a Sudamerica</t>
+  </si>
+  <si>
+    <t>la mas alta</t>
+  </si>
+  <si>
+    <t>Contexto externo</t>
+  </si>
+  <si>
+    <t>Negativo</t>
+  </si>
+  <si>
+    <t>Sectores de mayor crecimiento</t>
+  </si>
+  <si>
+    <t>Financieros, Construcción, Manufacturas</t>
+  </si>
+  <si>
+    <t>Impulsos de lado de la oferta</t>
+  </si>
+  <si>
+    <t>Sectores no extractivos</t>
+  </si>
+  <si>
+    <t>Demanda Interna, impulsos fiscales y monetarios</t>
+  </si>
+  <si>
+    <t>del lado del gasto</t>
+  </si>
+  <si>
+    <t>impulso Fiscal y Monetario</t>
+  </si>
+  <si>
+    <t>Por el lado de la demanda</t>
+  </si>
+  <si>
+    <t>Demanda interna</t>
+  </si>
+  <si>
+    <t>Consumo privado e Infraestructura</t>
+  </si>
+  <si>
+    <t>lado Fiscal</t>
+  </si>
+  <si>
+    <t>Mayor Inversión Pública</t>
+  </si>
+  <si>
+    <t>Tal vez poner PII para decir quiénes nos financian</t>
+  </si>
+  <si>
+    <t>Todos los sectores</t>
+  </si>
+  <si>
+    <t>Demanda Interna</t>
+  </si>
+  <si>
+    <t>Financieros destaca</t>
+  </si>
+  <si>
+    <t>Algo especial</t>
+  </si>
+  <si>
+    <t>Modelo de desarrollo basdo en la intervención estatal</t>
+  </si>
+  <si>
+    <t>Recuperación de la economía mundial</t>
+  </si>
+  <si>
+    <t>Actividades Extractivas</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>La niña afectó al sector agropecuario</t>
+  </si>
+  <si>
+    <t>San Cristobal no impulso tanto</t>
+  </si>
+  <si>
+    <t>Hidrocarburos por ventas a Brasil</t>
+  </si>
+  <si>
+    <t>destaca sectores no extractivos, y minería</t>
   </si>
 </sst>
 </file>
@@ -167,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -190,6 +281,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +605,9 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="8" t="s">
@@ -625,4 +722,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2005</v>
+      </c>
+      <c r="C3">
+        <v>2006</v>
+      </c>
+      <c r="D3">
+        <v>2007</v>
+      </c>
+      <c r="E3">
+        <v>2008</v>
+      </c>
+      <c r="F3">
+        <v>2009</v>
+      </c>
+      <c r="G3">
+        <v>2010</v>
+      </c>
+      <c r="H3">
+        <v>2011</v>
+      </c>
+      <c r="I3">
+        <v>2012</v>
+      </c>
+      <c r="J3">
+        <v>2013</v>
+      </c>
+      <c r="K3">
+        <v>2014</v>
+      </c>
+      <c r="L3">
+        <v>2015</v>
+      </c>
+      <c r="M3">
+        <v>2016</v>
+      </c>
+      <c r="N3">
+        <v>2017</v>
+      </c>
+      <c r="O3">
+        <v>2018</v>
+      </c>
+      <c r="P3">
+        <v>2019</v>
+      </c>
+      <c r="Q3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="9">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="J4" s="9">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M4" s="9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>